<commit_message>
results with 4 apaches and 50 cache dbs
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="11640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="48">
   <si>
     <t>Loading</t>
   </si>
@@ -150,6 +151,78 @@
       </rPr>
       <t>templates are enabled</t>
     </r>
+  </si>
+  <si>
+    <t>Django 1.3 QL is disabled</t>
+  </si>
+  <si>
+    <t>10 databases</t>
+  </si>
+  <si>
+    <t>1 database</t>
+  </si>
+  <si>
+    <t>Single report 50 users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Errors: </t>
+  </si>
+  <si>
+    <t>4 Apaches 10 databases</t>
+  </si>
+  <si>
+    <t>4 Apaches 1 database</t>
+  </si>
+  <si>
+    <t>4 Apaches 50 databases</t>
+  </si>
+  <si>
+    <t>50 databases</t>
+  </si>
+  <si>
+    <t>4 App 10 db</t>
+  </si>
+  <si>
+    <t>4 App 50 db</t>
+  </si>
+  <si>
+    <t>1 App 10 db</t>
+  </si>
+  <si>
+    <t>1 App 50 db</t>
+  </si>
+  <si>
+    <t>4 App 50 db 128 th in ch</t>
+  </si>
+  <si>
+    <t>1 App 50 db 128 in ch MAxRequest = 1</t>
+  </si>
+  <si>
+    <t>with static proccessed by proxy</t>
+  </si>
+  <si>
+    <t>1 App 50 db 4 listener &amp; virt dir</t>
+  </si>
+  <si>
+    <t>Test Case 6: 3 reports (From SharePoint settings - All Reports, Site Permissions, User Permissions), Site Collection Administrator</t>
+  </si>
+  <si>
+    <t>233 samples</t>
+  </si>
+  <si>
+    <t>All Reports</t>
+  </si>
+  <si>
+    <t>User Perm</t>
+  </si>
+  <si>
+    <t>Site Perm</t>
+  </si>
+  <si>
+    <t>1 User</t>
+  </si>
+  <si>
+    <t>1 Apache, 1 cache db</t>
   </si>
 </sst>
 </file>
@@ -194,9 +267,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,23 +444,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="61555072"/>
-        <c:axId val="61556608"/>
+        <c:axId val="77431168"/>
+        <c:axId val="77432704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61555072"/>
+        <c:axId val="77431168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61556608"/>
+        <c:crossAx val="77432704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61556608"/>
+        <c:axId val="77432704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -394,20 +468,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61555072"/>
+        <c:crossAx val="77431168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -961,7 +1034,7 @@
         <v>59223.040000000001</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F5:F8" si="4">E8/A8</f>
+        <f t="shared" ref="F8" si="4">E8/A8</f>
         <v>462.68</v>
       </c>
     </row>
@@ -1383,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2040,7 +2113,7 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" ref="F38:F41" si="13">E38/A38</f>
+        <f t="shared" ref="F38:F39" si="13">E38/A38</f>
         <v>0</v>
       </c>
       <c r="I38">
@@ -2209,7 +2282,7 @@
         <v>10</v>
       </c>
       <c r="E47">
-        <f t="shared" ref="E47:E49" si="16">B47+C47+C47+D47</f>
+        <f t="shared" ref="E47:E48" si="16">B47+C47+C47+D47</f>
         <v>0</v>
       </c>
       <c r="F47">
@@ -2326,12 +2399,539 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>34</v>
+      </c>
+      <c r="C6">
+        <v>375</v>
+      </c>
+      <c r="D6">
+        <v>3107</v>
+      </c>
+      <c r="E6">
+        <f>B6+C6+C6+D6</f>
+        <v>3891</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>176</v>
+      </c>
+      <c r="C7">
+        <v>5613</v>
+      </c>
+      <c r="D7">
+        <v>14040</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7" si="0">B7+C7+C7+D7</f>
+        <v>25442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>210</v>
+      </c>
+      <c r="C12">
+        <v>4830</v>
+      </c>
+      <c r="D12">
+        <v>10341</v>
+      </c>
+      <c r="E12">
+        <f>B12+C12+C12+D12</f>
+        <v>20211</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12">
+        <v>210</v>
+      </c>
+      <c r="J12">
+        <v>4830</v>
+      </c>
+      <c r="K12">
+        <v>10341</v>
+      </c>
+      <c r="L12">
+        <f>I12+J12+J12+K12</f>
+        <v>20211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="H13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13">
+        <v>197</v>
+      </c>
+      <c r="J13">
+        <v>5027</v>
+      </c>
+      <c r="K13">
+        <v>10648</v>
+      </c>
+      <c r="L13">
+        <f>I13+J13+J13+K13</f>
+        <v>20899</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14">
+        <v>285</v>
+      </c>
+      <c r="J14">
+        <v>1758</v>
+      </c>
+      <c r="K14">
+        <v>9334</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:L23" si="1">I14+J14+J14+K14</f>
+        <v>13135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15">
+        <v>295</v>
+      </c>
+      <c r="J15">
+        <v>1725</v>
+      </c>
+      <c r="K15">
+        <v>9570</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>13315</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <v>197</v>
+      </c>
+      <c r="C17">
+        <v>5027</v>
+      </c>
+      <c r="D17">
+        <v>10648</v>
+      </c>
+      <c r="E17">
+        <f>B17+C17+C17+D17</f>
+        <v>20899</v>
+      </c>
+      <c r="H17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17">
+        <v>365</v>
+      </c>
+      <c r="J17">
+        <v>1840</v>
+      </c>
+      <c r="K17">
+        <v>7645</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>11690</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19">
+        <v>1487</v>
+      </c>
+      <c r="J19">
+        <v>4987</v>
+      </c>
+      <c r="K19">
+        <v>8785</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>20246</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21">
+        <v>346</v>
+      </c>
+      <c r="J21">
+        <v>1602</v>
+      </c>
+      <c r="K21">
+        <v>7936</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>11486</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>50</v>
+      </c>
+      <c r="B22">
+        <v>230</v>
+      </c>
+      <c r="C22">
+        <v>4373</v>
+      </c>
+      <c r="D22">
+        <v>11075</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22" si="2">B22+C22+C22+D22</f>
+        <v>20051</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="H23" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23">
+        <v>213</v>
+      </c>
+      <c r="J23">
+        <v>4922</v>
+      </c>
+      <c r="K23">
+        <v>11204</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>21261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28">
+        <v>50</v>
+      </c>
+      <c r="B28">
+        <v>285</v>
+      </c>
+      <c r="C28">
+        <v>1758</v>
+      </c>
+      <c r="D28">
+        <v>9334</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ref="E28" si="3">B28+C28+C28+D28</f>
+        <v>13135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>50</v>
+      </c>
+      <c r="B33">
+        <v>295</v>
+      </c>
+      <c r="C33">
+        <v>1725</v>
+      </c>
+      <c r="D33">
+        <v>9570</v>
+      </c>
+      <c r="E33">
+        <f t="shared" ref="E33" si="4">B33+C33+C33+D33</f>
+        <v>13315</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>50</v>
+      </c>
+      <c r="B39">
+        <v>209</v>
+      </c>
+      <c r="C39">
+        <v>5222</v>
+      </c>
+      <c r="D39">
+        <v>6820</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ref="E39" si="5">B39+C39+C39+D39</f>
+        <v>17473</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9">
+        <v>14551</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added scripts for site permission report - 200 users and databases. And results.
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -4,20 +4,27 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="11640" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="11640" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Agnet and Broker" sheetId="5" r:id="rId5"/>
+    <sheet name="NewCore" sheetId="6" r:id="rId6"/>
+    <sheet name="Search" sheetId="7" r:id="rId7"/>
+    <sheet name="NoAsyncBroker" sheetId="8" r:id="rId8"/>
+    <sheet name="OneTimeRun" sheetId="10" r:id="rId9"/>
+    <sheet name="Sheet8" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="136">
   <si>
     <t>Loading</t>
   </si>
@@ -224,12 +231,279 @@
   <si>
     <t>1 Apache, 1 cache db</t>
   </si>
+  <si>
+    <t>Broker Site Permission Report</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>Single Production Site and Database</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>50 production databases</t>
+  </si>
+  <si>
+    <t>Cherrypy 128 threads</t>
+  </si>
+  <si>
+    <t>5% errors socket timout (200 sec)</t>
+  </si>
+  <si>
+    <t>Reqs / sec</t>
+  </si>
+  <si>
+    <t>18% errors</t>
+  </si>
+  <si>
+    <t>Agent (no logs 128 threads)</t>
+  </si>
+  <si>
+    <t>No logging:</t>
+  </si>
+  <si>
+    <t>0.27% errors request timeout</t>
+  </si>
+  <si>
+    <t>0,20%</t>
+  </si>
+  <si>
+    <t>0,19% request timeout</t>
+  </si>
+  <si>
+    <t>4 Agents + Apache as load balancer (500 threads and keepalive = on)</t>
+  </si>
+  <si>
+    <t>8 Agents + Apache as load balancer (500 threads and keepalive = on)</t>
+  </si>
+  <si>
+    <t>0,62% request timeout</t>
+  </si>
+  <si>
+    <t>0.29% errors request timeout</t>
+  </si>
+  <si>
+    <t>Via Broker:</t>
+  </si>
+  <si>
+    <t>Prod</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>1 report 4 Apaches 4 Abrokers</t>
+  </si>
+  <si>
+    <t>Cache 2</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>1 report 8 Apaches 4 Abrokers</t>
+  </si>
+  <si>
+    <t>1 report 16 Apaches 4 Abrokers</t>
+  </si>
+  <si>
+    <t>1 report 1 Apaches 4 Abrokers</t>
+  </si>
+  <si>
+    <t>50 reports 16 apaches 4 agent, brokers and asyncbrokers</t>
+  </si>
+  <si>
+    <t>New build 8 Apaches 4 other services</t>
+  </si>
+  <si>
+    <t>Embedded disabled</t>
+  </si>
+  <si>
+    <t>Single Report</t>
+  </si>
+  <si>
+    <t>0.31% of errors</t>
+  </si>
+  <si>
+    <t>Single Report with Embedded resources</t>
+  </si>
+  <si>
+    <t>Socket Errors start after these sample</t>
+  </si>
+  <si>
+    <t>Searching</t>
+  </si>
+  <si>
+    <t>Build 4.2.2.2002</t>
+  </si>
+  <si>
+    <t>1 Apache, 1 other services</t>
+  </si>
+  <si>
+    <t>50 users try to open his All Reports from SharEPoint site settings</t>
+  </si>
+  <si>
+    <t>&gt; 200 sec</t>
+  </si>
+  <si>
+    <t>~60 sec</t>
+  </si>
+  <si>
+    <t>8 apaches 4 others</t>
+  </si>
+  <si>
+    <t>Prod Max</t>
+  </si>
+  <si>
+    <t>Search Max</t>
+  </si>
+  <si>
+    <t>Loading Max</t>
+  </si>
+  <si>
+    <t>Total Max</t>
+  </si>
+  <si>
+    <t>Agent: Cannot read data from content database</t>
+  </si>
+  <si>
+    <t>Hang !!! And restored after 5 minutes</t>
+  </si>
+  <si>
+    <t>8 Apaches 1 other services</t>
+  </si>
+  <si>
+    <t>L Max</t>
+  </si>
+  <si>
+    <t>C Max</t>
+  </si>
+  <si>
+    <t>P Max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 Apaches 0 other services 5 sec sleep interval </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 Apaches 0 other services 5 sec sleep interval </t>
+  </si>
+  <si>
+    <t>Build  4.2.2.2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 Apaches 0 other services 1 sec sleep interval </t>
+  </si>
+  <si>
+    <t>No Async Broker</t>
+  </si>
+  <si>
+    <t>Build 2028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customizations: 5 threads in Broker and Agent, Cache for SQLalchemy, pool_size = 100, pool_timeout=300 </t>
+  </si>
+  <si>
+    <t>Every user see its own report</t>
+  </si>
+  <si>
+    <t>Opened reports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customizations: 10 threads in Broker and Agent, Cache for SQLalchemy, pool_size = 100, pool_timeout=300 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customizations: 64 threads in Broker and Agent, Cache for SQLalchemy, pool_size = 200, pool_timeout=300 </t>
+  </si>
+  <si>
+    <t>Errors !!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customizations: 20 threads in Broker and Agent, Cache for SQLalchemy, pool_size = 200, pool_timeout=300 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customizations: 10 threads in Broker and Agent, Cache for SQLalchemy, pool_size = 200, pool_timeout=300 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Apaches 0 other services 1 sec sleep interval </t>
+  </si>
+  <si>
+    <t>Apaches</t>
+  </si>
+  <si>
+    <t>10*20</t>
+  </si>
+  <si>
+    <t>Memory: 200 * 15 + 8 * 70 + 10 * 5 + 150 + 50</t>
+  </si>
+  <si>
+    <t>Total Report Views</t>
+  </si>
+  <si>
+    <t>Unique Users (=threads)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique reports </t>
+  </si>
+  <si>
+    <t>Avg Time</t>
+  </si>
+  <si>
+    <t>Max Time</t>
+  </si>
+  <si>
+    <t>Memory Usage</t>
+  </si>
+  <si>
+    <t>11 sec</t>
+  </si>
+  <si>
+    <t>65 sec</t>
+  </si>
+  <si>
+    <t>75 sec</t>
+  </si>
+  <si>
+    <t>550 sec</t>
+  </si>
+  <si>
+    <t>4 GB</t>
+  </si>
+  <si>
+    <t>1 GB</t>
+  </si>
+  <si>
+    <t>Build 2042. 8 apaches</t>
+  </si>
+  <si>
+    <t>One time report open</t>
+  </si>
+  <si>
+    <t>4 agents and 4 brokers</t>
+  </si>
+  <si>
+    <t>Continues</t>
+  </si>
+  <si>
+    <t>One Time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +513,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -267,10 +549,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,23 +738,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="77431168"/>
-        <c:axId val="77432704"/>
+        <c:axId val="62862848"/>
+        <c:axId val="62864384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77431168"/>
+        <c:axId val="62862848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77432704"/>
+        <c:crossAx val="62864384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77432704"/>
+        <c:axId val="62864384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -468,7 +762,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77431168"/>
+        <c:crossAx val="62862848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -480,7 +774,151 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
+    <c:title/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Agnet and Broker'!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Agnet and Broker'!$A$7:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Agnet and Broker'!$B$7:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>693</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1158</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3614</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9136</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18169</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34570</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32697</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>79224</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>147174</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="62220928"/>
+        <c:axId val="64123264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="62220928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64123264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="64123264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="62220928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -504,6 +942,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1452,6 +1925,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N50"/>
@@ -2402,7 +2887,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2456,6 +2941,10 @@
         <f>B6+C6+C6+D6</f>
         <v>3891</v>
       </c>
+      <c r="F6">
+        <f>1000*A6/B6</f>
+        <v>29.411764705882351</v>
+      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
@@ -2473,6 +2962,10 @@
       <c r="E7">
         <f t="shared" ref="E7" si="0">B7+C7+C7+D7</f>
         <v>25442</v>
+      </c>
+      <c r="F7">
+        <f>1000*A7/B7</f>
+        <v>284.09090909090907</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2879,7 +3372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2934,4 +3427,3466 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="15.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="K3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>693</v>
+      </c>
+      <c r="C7" s="5">
+        <f t="shared" ref="C7:C16" si="0">A7*1000/B7</f>
+        <v>1.4430014430014431</v>
+      </c>
+      <c r="D7">
+        <v>670</v>
+      </c>
+      <c r="E7">
+        <v>980</v>
+      </c>
+      <c r="F7">
+        <v>112</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <v>638</v>
+      </c>
+      <c r="M7" s="5">
+        <f>K7*1000/L7</f>
+        <v>1.567398119122257</v>
+      </c>
+      <c r="N7">
+        <v>688</v>
+      </c>
+      <c r="O7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1158</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" si="0"/>
+        <v>4.3177892918825558</v>
+      </c>
+      <c r="D8">
+        <v>711</v>
+      </c>
+      <c r="E8">
+        <v>2246</v>
+      </c>
+      <c r="F8">
+        <v>523</v>
+      </c>
+      <c r="K8" s="2">
+        <v>5</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="2">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2049</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" si="0"/>
+        <v>4.8804294777940456</v>
+      </c>
+      <c r="D9">
+        <v>643</v>
+      </c>
+      <c r="E9">
+        <v>3037</v>
+      </c>
+      <c r="F9">
+        <v>694</v>
+      </c>
+      <c r="K9" s="2">
+        <v>10</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="2">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3614</v>
+      </c>
+      <c r="C10" s="5">
+        <f t="shared" si="0"/>
+        <v>5.5340343110127286</v>
+      </c>
+      <c r="D10">
+        <v>1139</v>
+      </c>
+      <c r="E10">
+        <v>5587</v>
+      </c>
+      <c r="F10">
+        <v>846</v>
+      </c>
+      <c r="K10" s="2">
+        <v>20</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="2">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2">
+        <v>9136</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" si="0"/>
+        <v>5.4728546409807359</v>
+      </c>
+      <c r="D11">
+        <v>705</v>
+      </c>
+      <c r="E11">
+        <v>10641</v>
+      </c>
+      <c r="F11">
+        <v>1030</v>
+      </c>
+      <c r="K11" s="2">
+        <v>50</v>
+      </c>
+      <c r="L11" s="2">
+        <v>5582</v>
+      </c>
+      <c r="M11" s="5">
+        <f>K11*1000/L11</f>
+        <v>8.9573629523468288</v>
+      </c>
+      <c r="N11">
+        <v>7966</v>
+      </c>
+      <c r="O11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="2">
+        <v>100</v>
+      </c>
+      <c r="B12" s="2">
+        <v>18169</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="0"/>
+        <v>5.5038802355660739</v>
+      </c>
+      <c r="D12">
+        <v>1204</v>
+      </c>
+      <c r="E12">
+        <v>20510</v>
+      </c>
+      <c r="F12">
+        <v>1484</v>
+      </c>
+      <c r="K12" s="2">
+        <v>100</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="2">
+        <v>200</v>
+      </c>
+      <c r="B13" s="2">
+        <v>34570</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" si="0"/>
+        <v>5.7853630315302285</v>
+      </c>
+      <c r="D13">
+        <v>2165</v>
+      </c>
+      <c r="E13">
+        <v>200000</v>
+      </c>
+      <c r="F13">
+        <v>1149</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="2">
+        <v>200</v>
+      </c>
+      <c r="L13" s="2">
+        <v>26083</v>
+      </c>
+      <c r="M13" s="5">
+        <f t="shared" ref="M13:M15" si="1">K13*1000/L13</f>
+        <v>7.6678296208258256</v>
+      </c>
+      <c r="N13">
+        <v>130699</v>
+      </c>
+      <c r="O13">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="2">
+        <v>200</v>
+      </c>
+      <c r="B14" s="2">
+        <v>32697</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="0"/>
+        <v>6.1167691225494698</v>
+      </c>
+      <c r="D14">
+        <v>9812</v>
+      </c>
+      <c r="E14">
+        <v>114443</v>
+      </c>
+      <c r="F14">
+        <v>675</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>500</v>
+      </c>
+      <c r="L14" s="2">
+        <v>66452</v>
+      </c>
+      <c r="M14" s="5">
+        <f t="shared" si="1"/>
+        <v>7.5242280142057423</v>
+      </c>
+      <c r="N14">
+        <v>294801</v>
+      </c>
+      <c r="O14">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="2">
+        <v>500</v>
+      </c>
+      <c r="B15" s="2">
+        <v>79224</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" si="0"/>
+        <v>6.3112188225790167</v>
+      </c>
+      <c r="D15">
+        <v>6708</v>
+      </c>
+      <c r="E15">
+        <v>267805</v>
+      </c>
+      <c r="F15">
+        <v>1507</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1000</v>
+      </c>
+      <c r="L15" s="2">
+        <v>123403</v>
+      </c>
+      <c r="M15" s="5">
+        <f t="shared" si="1"/>
+        <v>8.10353070832962</v>
+      </c>
+      <c r="N15">
+        <v>375476</v>
+      </c>
+      <c r="O15">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B16" s="2">
+        <v>147174</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" si="0"/>
+        <v>6.7946784078709559</v>
+      </c>
+      <c r="D16">
+        <v>6273</v>
+      </c>
+      <c r="E16">
+        <v>400000</v>
+      </c>
+      <c r="F16">
+        <v>2539</v>
+      </c>
+      <c r="G16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="K18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" t="s">
+        <v>51</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M20" t="s">
+        <v>57</v>
+      </c>
+      <c r="N20" t="s">
+        <v>53</v>
+      </c>
+      <c r="O20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="K21" s="2">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2">
+        <v>525</v>
+      </c>
+      <c r="M21" s="5">
+        <f>K21*1000/L21</f>
+        <v>1.9047619047619047</v>
+      </c>
+      <c r="N21">
+        <v>1097</v>
+      </c>
+      <c r="O21">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="2">
+        <v>5</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="K22" s="2">
+        <v>5</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="2">
+        <v>10</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="K23" s="2">
+        <v>10</v>
+      </c>
+      <c r="L23" s="2"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="2">
+        <v>20</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="K24" s="2">
+        <v>20</v>
+      </c>
+      <c r="L24" s="2"/>
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="2">
+        <v>50</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="K25" s="2">
+        <v>50</v>
+      </c>
+      <c r="L25" s="2">
+        <v>2173</v>
+      </c>
+      <c r="M25" s="5">
+        <f>K25*1000/L25</f>
+        <v>23.00966405890474</v>
+      </c>
+      <c r="N25">
+        <v>3191</v>
+      </c>
+      <c r="O25">
+        <v>1458</v>
+      </c>
+      <c r="P25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="2">
+        <v>100</v>
+      </c>
+      <c r="B26" s="2">
+        <v>13870</v>
+      </c>
+      <c r="C26" s="5">
+        <f>A26*1000/B26</f>
+        <v>7.2098053352559477</v>
+      </c>
+      <c r="D26">
+        <v>853</v>
+      </c>
+      <c r="E26">
+        <v>17296</v>
+      </c>
+      <c r="F26">
+        <v>1418</v>
+      </c>
+      <c r="K26" s="2">
+        <v>100</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="2">
+        <v>200</v>
+      </c>
+      <c r="B27" s="2">
+        <v>26493</v>
+      </c>
+      <c r="C27" s="5">
+        <f>A27*1000/B27</f>
+        <v>7.5491639300947417</v>
+      </c>
+      <c r="D27">
+        <v>1442</v>
+      </c>
+      <c r="E27">
+        <v>121211</v>
+      </c>
+      <c r="F27">
+        <v>902</v>
+      </c>
+      <c r="K27" s="2">
+        <v>200</v>
+      </c>
+      <c r="L27" s="2">
+        <v>8242</v>
+      </c>
+      <c r="M27" s="5">
+        <f t="shared" ref="M27:M29" si="2">K27*1000/L27</f>
+        <v>24.265954865323952</v>
+      </c>
+      <c r="O27">
+        <v>1977</v>
+      </c>
+      <c r="P27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="2">
+        <v>500</v>
+      </c>
+      <c r="B28" s="2">
+        <v>62810</v>
+      </c>
+      <c r="C28" s="5">
+        <f t="shared" ref="C28:C29" si="3">A28*1000/B28</f>
+        <v>7.960515841426524</v>
+      </c>
+      <c r="D28">
+        <v>2139</v>
+      </c>
+      <c r="E28">
+        <v>212681</v>
+      </c>
+      <c r="F28">
+        <v>1527</v>
+      </c>
+      <c r="K28" s="2">
+        <v>500</v>
+      </c>
+      <c r="L28" s="2">
+        <v>19208</v>
+      </c>
+      <c r="M28" s="5">
+        <f t="shared" si="2"/>
+        <v>26.030820491461892</v>
+      </c>
+      <c r="N28">
+        <v>79097</v>
+      </c>
+      <c r="O28">
+        <v>2140</v>
+      </c>
+      <c r="P28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B29" s="2">
+        <v>126695</v>
+      </c>
+      <c r="C29" s="5">
+        <f t="shared" si="3"/>
+        <v>7.8929713090492912</v>
+      </c>
+      <c r="D29">
+        <v>9679</v>
+      </c>
+      <c r="E29">
+        <v>400000</v>
+      </c>
+      <c r="F29">
+        <v>2743</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1000</v>
+      </c>
+      <c r="L29" s="2"/>
+      <c r="M29" s="5" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="K32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="C33" s="5"/>
+      <c r="R33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" t="s">
+        <v>51</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M34" t="s">
+        <v>57</v>
+      </c>
+      <c r="N34" t="s">
+        <v>53</v>
+      </c>
+      <c r="O34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" s="2">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2">
+        <v>693</v>
+      </c>
+      <c r="C35" s="5">
+        <f t="shared" ref="C35:C39" si="4">A35*1000/B35</f>
+        <v>1.4430014430014431</v>
+      </c>
+      <c r="D35">
+        <v>670</v>
+      </c>
+      <c r="E35">
+        <v>980</v>
+      </c>
+      <c r="F35">
+        <v>112</v>
+      </c>
+      <c r="K35" s="2">
+        <v>1</v>
+      </c>
+      <c r="L35" s="2"/>
+      <c r="M35" s="5"/>
+      <c r="R35" s="2">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" s="2">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1158</v>
+      </c>
+      <c r="C36" s="5">
+        <f t="shared" si="4"/>
+        <v>4.3177892918825558</v>
+      </c>
+      <c r="D36">
+        <v>851</v>
+      </c>
+      <c r="E36">
+        <v>4092</v>
+      </c>
+      <c r="F36">
+        <v>535</v>
+      </c>
+      <c r="K36" s="2">
+        <v>5</v>
+      </c>
+      <c r="L36" s="2"/>
+      <c r="M36" s="5"/>
+      <c r="R36" s="2"/>
+    </row>
+    <row r="37" spans="1:19">
+      <c r="A37" s="2">
+        <v>10</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2180</v>
+      </c>
+      <c r="C37" s="5">
+        <f t="shared" si="4"/>
+        <v>4.5871559633027523</v>
+      </c>
+      <c r="D37">
+        <v>1536</v>
+      </c>
+      <c r="E37">
+        <v>4618</v>
+      </c>
+      <c r="F37">
+        <v>1229</v>
+      </c>
+      <c r="K37" s="2">
+        <v>10</v>
+      </c>
+      <c r="L37" s="2"/>
+      <c r="M37" s="5"/>
+      <c r="R37" s="2"/>
+    </row>
+    <row r="38" spans="1:19">
+      <c r="A38" s="2">
+        <v>20</v>
+      </c>
+      <c r="B38" s="2">
+        <v>3855</v>
+      </c>
+      <c r="C38" s="5">
+        <f t="shared" si="4"/>
+        <v>5.1880674448767836</v>
+      </c>
+      <c r="D38">
+        <v>2573</v>
+      </c>
+      <c r="E38">
+        <v>4932</v>
+      </c>
+      <c r="F38">
+        <v>892</v>
+      </c>
+      <c r="K38" s="2">
+        <v>20</v>
+      </c>
+      <c r="L38" s="2"/>
+      <c r="M38" s="5"/>
+      <c r="R38" s="2"/>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="A39" s="2">
+        <v>50</v>
+      </c>
+      <c r="B39" s="2">
+        <v>9894</v>
+      </c>
+      <c r="C39" s="5">
+        <f t="shared" si="4"/>
+        <v>5.0535678188801292</v>
+      </c>
+      <c r="D39">
+        <v>7015</v>
+      </c>
+      <c r="E39">
+        <v>11366</v>
+      </c>
+      <c r="F39">
+        <v>1034</v>
+      </c>
+      <c r="K39" s="2">
+        <v>50</v>
+      </c>
+      <c r="L39" s="2">
+        <v>1676</v>
+      </c>
+      <c r="M39" s="5">
+        <f>K39*1000/L39</f>
+        <v>29.832935560859188</v>
+      </c>
+      <c r="N39">
+        <v>3524</v>
+      </c>
+      <c r="O39">
+        <v>1036</v>
+      </c>
+      <c r="P39" t="s">
+        <v>67</v>
+      </c>
+      <c r="R39" s="2">
+        <v>6918</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
+      <c r="A40" s="2">
+        <v>100</v>
+      </c>
+      <c r="K40" s="2">
+        <v>100</v>
+      </c>
+      <c r="L40" s="2"/>
+      <c r="M40" s="5"/>
+      <c r="R40" s="2"/>
+    </row>
+    <row r="41" spans="1:19">
+      <c r="K41" s="2">
+        <v>200</v>
+      </c>
+      <c r="L41" s="2"/>
+      <c r="M41" s="5"/>
+      <c r="R41" s="2">
+        <v>26845</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="K42" s="2">
+        <v>500</v>
+      </c>
+      <c r="L42" s="2">
+        <v>15661</v>
+      </c>
+      <c r="M42" s="5">
+        <f t="shared" ref="M42" si="5">K42*1000/L42</f>
+        <v>31.926441478832768</v>
+      </c>
+      <c r="N42">
+        <v>20771</v>
+      </c>
+      <c r="O42">
+        <v>2413</v>
+      </c>
+      <c r="P42" t="s">
+        <v>66</v>
+      </c>
+      <c r="R42" s="2">
+        <v>55563</v>
+      </c>
+      <c r="S42" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
+      <c r="K43" s="2">
+        <v>1000</v>
+      </c>
+      <c r="L43" s="2"/>
+      <c r="M43" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:V38"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14:V18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="J1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>72</v>
+      </c>
+      <c r="O4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5">
+        <v>200</v>
+      </c>
+      <c r="B5">
+        <v>5138</v>
+      </c>
+      <c r="C5">
+        <v>694</v>
+      </c>
+      <c r="D5">
+        <v>47450</v>
+      </c>
+      <c r="E5">
+        <v>48301</v>
+      </c>
+      <c r="F5">
+        <v>2450</v>
+      </c>
+      <c r="G5">
+        <v>2321</v>
+      </c>
+      <c r="H5">
+        <f>C5+D5+E5+F5</f>
+        <v>98895</v>
+      </c>
+      <c r="J5">
+        <v>50</v>
+      </c>
+      <c r="K5">
+        <v>90000</v>
+      </c>
+      <c r="L5">
+        <v>32</v>
+      </c>
+      <c r="M5">
+        <v>894</v>
+      </c>
+      <c r="N5">
+        <v>728</v>
+      </c>
+      <c r="O5">
+        <v>2570</v>
+      </c>
+      <c r="P5">
+        <v>34</v>
+      </c>
+      <c r="Q5">
+        <f>L5+M5+N5+O5</f>
+        <v>4224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="J6">
+        <v>200</v>
+      </c>
+      <c r="K6">
+        <v>13750</v>
+      </c>
+      <c r="L6">
+        <v>48</v>
+      </c>
+      <c r="M6">
+        <v>6610</v>
+      </c>
+      <c r="N6">
+        <v>4920</v>
+      </c>
+      <c r="O6">
+        <v>5000</v>
+      </c>
+      <c r="P6">
+        <v>79</v>
+      </c>
+      <c r="Q6">
+        <f>L6+M6+N6+O6</f>
+        <v>16578</v>
+      </c>
+      <c r="R6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>70</v>
+      </c>
+      <c r="S10" t="s">
+        <v>98</v>
+      </c>
+      <c r="T10" t="s">
+        <v>99</v>
+      </c>
+      <c r="U10" t="s">
+        <v>100</v>
+      </c>
+      <c r="V10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11">
+        <v>200</v>
+      </c>
+      <c r="B11">
+        <v>10164</v>
+      </c>
+      <c r="C11">
+        <v>314</v>
+      </c>
+      <c r="D11">
+        <v>7738</v>
+      </c>
+      <c r="E11">
+        <v>7896</v>
+      </c>
+      <c r="F11">
+        <v>1543</v>
+      </c>
+      <c r="G11">
+        <v>1345</v>
+      </c>
+      <c r="H11">
+        <f>C11+D11+E11+F11</f>
+        <v>17491</v>
+      </c>
+      <c r="J11">
+        <v>50</v>
+      </c>
+      <c r="K11">
+        <v>65986</v>
+      </c>
+      <c r="L11">
+        <v>14</v>
+      </c>
+      <c r="M11">
+        <v>217</v>
+      </c>
+      <c r="N11">
+        <v>658</v>
+      </c>
+      <c r="O11">
+        <v>8776</v>
+      </c>
+      <c r="P11">
+        <v>12</v>
+      </c>
+      <c r="Q11">
+        <f>L11+M11+N11+O11</f>
+        <v>9665</v>
+      </c>
+      <c r="S11">
+        <v>2458</v>
+      </c>
+      <c r="T11">
+        <v>30275</v>
+      </c>
+      <c r="U11">
+        <v>27417</v>
+      </c>
+      <c r="V11">
+        <f>S11+U11+T11*2</f>
+        <v>90425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="J12">
+        <v>200</v>
+      </c>
+      <c r="Q12">
+        <f>L12+M12+N12+O12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="J14" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16">
+        <v>200</v>
+      </c>
+      <c r="B16">
+        <v>10264</v>
+      </c>
+      <c r="C16">
+        <v>198</v>
+      </c>
+      <c r="D16">
+        <v>4412</v>
+      </c>
+      <c r="E16">
+        <v>4393</v>
+      </c>
+      <c r="F16">
+        <v>708</v>
+      </c>
+      <c r="G16">
+        <v>501</v>
+      </c>
+      <c r="H16">
+        <f>C16+D16+E16+F16</f>
+        <v>9711</v>
+      </c>
+      <c r="J16" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L16" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" t="s">
+        <v>72</v>
+      </c>
+      <c r="O16" t="s">
+        <v>69</v>
+      </c>
+      <c r="P16" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>70</v>
+      </c>
+      <c r="S16" t="s">
+        <v>98</v>
+      </c>
+      <c r="T16" t="s">
+        <v>99</v>
+      </c>
+      <c r="U16" t="s">
+        <v>100</v>
+      </c>
+      <c r="V16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="J17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18">
+        <v>200</v>
+      </c>
+      <c r="K18">
+        <v>29191</v>
+      </c>
+      <c r="L18">
+        <v>57</v>
+      </c>
+      <c r="M18">
+        <v>4151</v>
+      </c>
+      <c r="N18">
+        <v>3740</v>
+      </c>
+      <c r="O18">
+        <v>5286</v>
+      </c>
+      <c r="P18">
+        <v>151</v>
+      </c>
+      <c r="Q18">
+        <f>L18+M18+N18+O18</f>
+        <v>13234</v>
+      </c>
+      <c r="S18">
+        <v>3441</v>
+      </c>
+      <c r="T18">
+        <v>34708</v>
+      </c>
+      <c r="U18">
+        <v>30209</v>
+      </c>
+      <c r="V18">
+        <f>S18+U18+T18*2</f>
+        <v>103066</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" t="s">
+        <v>70</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21">
+        <v>200</v>
+      </c>
+      <c r="B21">
+        <v>10604</v>
+      </c>
+      <c r="C21">
+        <v>203</v>
+      </c>
+      <c r="D21">
+        <v>2472</v>
+      </c>
+      <c r="E21">
+        <v>2541</v>
+      </c>
+      <c r="F21">
+        <v>431</v>
+      </c>
+      <c r="G21">
+        <v>89</v>
+      </c>
+      <c r="H21">
+        <f>C21+D21+E21+F21</f>
+        <v>5647</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="A22">
+        <v>300</v>
+      </c>
+      <c r="B22">
+        <v>15898</v>
+      </c>
+      <c r="C22">
+        <v>468</v>
+      </c>
+      <c r="D22">
+        <v>4256</v>
+      </c>
+      <c r="E22">
+        <v>4333</v>
+      </c>
+      <c r="F22">
+        <v>459</v>
+      </c>
+      <c r="G22">
+        <v>99</v>
+      </c>
+      <c r="H22">
+        <f>C22+D22+E22+F22</f>
+        <v>9516</v>
+      </c>
+      <c r="J22" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" t="s">
+        <v>51</v>
+      </c>
+      <c r="L22" t="s">
+        <v>0</v>
+      </c>
+      <c r="M22" t="s">
+        <v>1</v>
+      </c>
+      <c r="N22" t="s">
+        <v>72</v>
+      </c>
+      <c r="O22" t="s">
+        <v>69</v>
+      </c>
+      <c r="P22" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>70</v>
+      </c>
+      <c r="S22" t="s">
+        <v>98</v>
+      </c>
+      <c r="T22" t="s">
+        <v>99</v>
+      </c>
+      <c r="U22" t="s">
+        <v>100</v>
+      </c>
+      <c r="V22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="J23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="J24">
+        <v>200</v>
+      </c>
+      <c r="K24">
+        <v>43832</v>
+      </c>
+      <c r="L24">
+        <v>12</v>
+      </c>
+      <c r="M24">
+        <v>489</v>
+      </c>
+      <c r="N24">
+        <v>853</v>
+      </c>
+      <c r="O24">
+        <v>13421</v>
+      </c>
+      <c r="P24">
+        <v>22</v>
+      </c>
+      <c r="Q24">
+        <f>L24+M24+N24+O24</f>
+        <v>14775</v>
+      </c>
+      <c r="S24">
+        <v>1138</v>
+      </c>
+      <c r="T24">
+        <v>25321</v>
+      </c>
+      <c r="U24">
+        <v>53311</v>
+      </c>
+      <c r="V24">
+        <f>S24+U24+T24*2</f>
+        <v>105091</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22">
+      <c r="A27">
+        <v>50</v>
+      </c>
+      <c r="C27">
+        <v>122</v>
+      </c>
+      <c r="D27">
+        <v>1019</v>
+      </c>
+      <c r="E27">
+        <v>997</v>
+      </c>
+      <c r="F27">
+        <v>2266</v>
+      </c>
+      <c r="G27">
+        <v>29</v>
+      </c>
+      <c r="H27">
+        <f>C27+D27+E27+F27</f>
+        <v>4404</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22">
+      <c r="A28">
+        <v>200</v>
+      </c>
+      <c r="H28">
+        <f>C28+D28+E28+F28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
+      <c r="J29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
+      <c r="J30" t="s">
+        <v>5</v>
+      </c>
+      <c r="K30" t="s">
+        <v>51</v>
+      </c>
+      <c r="L30" t="s">
+        <v>0</v>
+      </c>
+      <c r="M30" t="s">
+        <v>1</v>
+      </c>
+      <c r="N30" t="s">
+        <v>72</v>
+      </c>
+      <c r="O30" t="s">
+        <v>69</v>
+      </c>
+      <c r="P30" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22">
+      <c r="Q31">
+        <f>L31+M31+N31+O31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22">
+      <c r="J32">
+        <v>500</v>
+      </c>
+      <c r="K32">
+        <v>71744</v>
+      </c>
+      <c r="L32">
+        <v>728</v>
+      </c>
+      <c r="M32">
+        <v>11565</v>
+      </c>
+      <c r="N32">
+        <v>10493</v>
+      </c>
+      <c r="O32">
+        <v>1861</v>
+      </c>
+      <c r="P32">
+        <v>1049</v>
+      </c>
+      <c r="Q32">
+        <f>L32+M32+N32+O32</f>
+        <v>24647</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="10:18">
+      <c r="J35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="10:18">
+      <c r="J36" t="s">
+        <v>5</v>
+      </c>
+      <c r="K36" t="s">
+        <v>51</v>
+      </c>
+      <c r="L36" t="s">
+        <v>0</v>
+      </c>
+      <c r="M36" t="s">
+        <v>1</v>
+      </c>
+      <c r="N36" t="s">
+        <v>72</v>
+      </c>
+      <c r="O36" t="s">
+        <v>69</v>
+      </c>
+      <c r="P36" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="10:18">
+      <c r="Q37">
+        <f>L37+M37+N37+O37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="10:18">
+      <c r="J38">
+        <v>500</v>
+      </c>
+      <c r="K38">
+        <v>49014</v>
+      </c>
+      <c r="L38">
+        <v>292</v>
+      </c>
+      <c r="M38">
+        <v>14823</v>
+      </c>
+      <c r="N38">
+        <v>14068</v>
+      </c>
+      <c r="O38">
+        <v>2282</v>
+      </c>
+      <c r="P38">
+        <v>909</v>
+      </c>
+      <c r="Q38">
+        <f>L38+M38+N38+O38</f>
+        <v>31465</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>12708</v>
+      </c>
+      <c r="C13">
+        <v>363</v>
+      </c>
+      <c r="D13">
+        <v>2796</v>
+      </c>
+      <c r="E13">
+        <v>5790</v>
+      </c>
+      <c r="F13">
+        <f>C13+D13+E13</f>
+        <v>8949</v>
+      </c>
+      <c r="H13">
+        <v>8153</v>
+      </c>
+      <c r="I13">
+        <v>25019</v>
+      </c>
+      <c r="J13">
+        <v>32240</v>
+      </c>
+      <c r="K13">
+        <f>H13+I13+J13</f>
+        <v>65412</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14">
+        <v>200</v>
+      </c>
+      <c r="B14">
+        <v>6843</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>8382</v>
+      </c>
+      <c r="E14">
+        <v>45034</v>
+      </c>
+      <c r="F14">
+        <f>C14+D14+E14</f>
+        <v>53426</v>
+      </c>
+      <c r="H14">
+        <v>188</v>
+      </c>
+      <c r="I14">
+        <v>108169</v>
+      </c>
+      <c r="J14">
+        <v>122713</v>
+      </c>
+      <c r="K14">
+        <f>H14+I14+J14</f>
+        <v>231070</v>
+      </c>
+      <c r="M14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15">
+        <v>500</v>
+      </c>
+      <c r="B15">
+        <v>6142</v>
+      </c>
+      <c r="C15">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>22434</v>
+      </c>
+      <c r="E15">
+        <v>70682</v>
+      </c>
+      <c r="F15">
+        <f>C15+D15+E15</f>
+        <v>93132</v>
+      </c>
+      <c r="H15">
+        <v>303</v>
+      </c>
+      <c r="I15">
+        <v>262174</v>
+      </c>
+      <c r="J15">
+        <v>200506</v>
+      </c>
+      <c r="K15">
+        <f>H15+I15+J15</f>
+        <v>462983</v>
+      </c>
+      <c r="M15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U75"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="6" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" style="6" customWidth="1"/>
+    <col min="21" max="21" width="16" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14">
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14">
+      <c r="B3" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
+      <c r="B4" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L6" t="s">
+        <v>99</v>
+      </c>
+      <c r="M6" t="s">
+        <v>100</v>
+      </c>
+      <c r="N6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
+      <c r="B7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
+      <c r="B8">
+        <v>200</v>
+      </c>
+      <c r="C8">
+        <v>20076</v>
+      </c>
+      <c r="D8">
+        <v>88</v>
+      </c>
+      <c r="E8">
+        <v>2435</v>
+      </c>
+      <c r="F8">
+        <v>1842</v>
+      </c>
+      <c r="G8">
+        <v>8378</v>
+      </c>
+      <c r="H8">
+        <v>25</v>
+      </c>
+      <c r="I8">
+        <f>D8+E8+F8+G8</f>
+        <v>12743</v>
+      </c>
+      <c r="K8">
+        <v>3879</v>
+      </c>
+      <c r="L8">
+        <v>31667</v>
+      </c>
+      <c r="M8">
+        <v>30529</v>
+      </c>
+      <c r="N8">
+        <f>K8+M8+L8*2</f>
+        <v>97742</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="B9">
+        <v>500</v>
+      </c>
+      <c r="C9">
+        <v>45135</v>
+      </c>
+      <c r="D9">
+        <v>116</v>
+      </c>
+      <c r="E9">
+        <v>9268</v>
+      </c>
+      <c r="F9">
+        <v>9825</v>
+      </c>
+      <c r="G9">
+        <v>5262</v>
+      </c>
+      <c r="H9">
+        <v>91</v>
+      </c>
+      <c r="I9">
+        <f>D9+E9+F9+G9</f>
+        <v>24471</v>
+      </c>
+      <c r="K9">
+        <v>1156</v>
+      </c>
+      <c r="L9">
+        <v>50185</v>
+      </c>
+      <c r="M9">
+        <v>25064</v>
+      </c>
+      <c r="N9">
+        <f>K9+M9+L9*2</f>
+        <v>126590</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14">
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14">
+      <c r="B14" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14">
+      <c r="B15" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14">
+      <c r="B16" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="B17" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" t="s">
+        <v>70</v>
+      </c>
+      <c r="K19" t="s">
+        <v>98</v>
+      </c>
+      <c r="L19" t="s">
+        <v>99</v>
+      </c>
+      <c r="M19" t="s">
+        <v>100</v>
+      </c>
+      <c r="N19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
+      <c r="B21">
+        <v>100</v>
+      </c>
+      <c r="C21">
+        <v>2090</v>
+      </c>
+      <c r="D21">
+        <v>142</v>
+      </c>
+      <c r="E21">
+        <v>3715</v>
+      </c>
+      <c r="F21">
+        <v>2639</v>
+      </c>
+      <c r="G21">
+        <v>27620</v>
+      </c>
+      <c r="H21">
+        <v>6</v>
+      </c>
+      <c r="I21">
+        <f>D21+E21+F21+G21</f>
+        <v>34116</v>
+      </c>
+      <c r="K21">
+        <v>2955</v>
+      </c>
+      <c r="L21">
+        <v>138970</v>
+      </c>
+      <c r="M21">
+        <v>138970</v>
+      </c>
+      <c r="N21">
+        <f>K21+M21+L21*2</f>
+        <v>419865</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="B22">
+        <v>500</v>
+      </c>
+      <c r="I22">
+        <f>D22+E22+F22+G22</f>
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f>K22+M22+L22*2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="B25" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14">
+      <c r="B27" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="B28" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" t="s">
+        <v>70</v>
+      </c>
+      <c r="K30" t="s">
+        <v>98</v>
+      </c>
+      <c r="L30" t="s">
+        <v>99</v>
+      </c>
+      <c r="M30" t="s">
+        <v>100</v>
+      </c>
+      <c r="N30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
+      <c r="B31">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14">
+      <c r="B32">
+        <v>100</v>
+      </c>
+      <c r="C32">
+        <v>2627</v>
+      </c>
+      <c r="D32">
+        <v>19</v>
+      </c>
+      <c r="E32">
+        <v>2230</v>
+      </c>
+      <c r="F32">
+        <v>1465</v>
+      </c>
+      <c r="G32">
+        <v>17747</v>
+      </c>
+      <c r="H32">
+        <v>7</v>
+      </c>
+      <c r="I32">
+        <f>D32+E32+F32+G32</f>
+        <v>21461</v>
+      </c>
+      <c r="K32">
+        <v>751</v>
+      </c>
+      <c r="L32">
+        <v>104085</v>
+      </c>
+      <c r="M32">
+        <v>98007</v>
+      </c>
+      <c r="N32">
+        <f>K32+M32+L32*2</f>
+        <v>306928</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="B33">
+        <v>100</v>
+      </c>
+      <c r="C33">
+        <v>4925</v>
+      </c>
+      <c r="D33">
+        <v>67</v>
+      </c>
+      <c r="E33">
+        <v>1444</v>
+      </c>
+      <c r="F33">
+        <v>1451</v>
+      </c>
+      <c r="G33">
+        <v>16924</v>
+      </c>
+      <c r="H33">
+        <v>7</v>
+      </c>
+      <c r="I33">
+        <f>D33+E33+F33+G33</f>
+        <v>19886</v>
+      </c>
+      <c r="K33">
+        <v>3178</v>
+      </c>
+      <c r="L33">
+        <v>109012</v>
+      </c>
+      <c r="M33">
+        <v>93060</v>
+      </c>
+      <c r="N33">
+        <f>K33+M33+L33*2</f>
+        <v>314262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="B34">
+        <v>200</v>
+      </c>
+      <c r="C34">
+        <v>8049</v>
+      </c>
+      <c r="D34">
+        <v>9</v>
+      </c>
+      <c r="E34">
+        <v>2424</v>
+      </c>
+      <c r="F34">
+        <v>7230</v>
+      </c>
+      <c r="G34">
+        <v>46768</v>
+      </c>
+      <c r="H34">
+        <v>10</v>
+      </c>
+      <c r="I34">
+        <f>D34+E34+F34+G34</f>
+        <v>56431</v>
+      </c>
+      <c r="K34">
+        <v>998</v>
+      </c>
+      <c r="L34">
+        <v>183356</v>
+      </c>
+      <c r="M34">
+        <v>177777</v>
+      </c>
+      <c r="N34">
+        <f>K34+M34+L34*2</f>
+        <v>545487</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
+      <c r="B36" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="B37" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="B38" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="B39" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="30" customHeight="1">
+      <c r="A41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>72</v>
+      </c>
+      <c r="G41" t="s">
+        <v>69</v>
+      </c>
+      <c r="H41" t="s">
+        <v>73</v>
+      </c>
+      <c r="I41" t="s">
+        <v>70</v>
+      </c>
+      <c r="K41" t="s">
+        <v>98</v>
+      </c>
+      <c r="L41" t="s">
+        <v>99</v>
+      </c>
+      <c r="M41" t="s">
+        <v>100</v>
+      </c>
+      <c r="N41" t="s">
+        <v>94</v>
+      </c>
+      <c r="P41" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q41" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="R41" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="S41" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="T41" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="U41" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>50</v>
+      </c>
+      <c r="C42">
+        <v>2109</v>
+      </c>
+      <c r="D42">
+        <v>7</v>
+      </c>
+      <c r="E42">
+        <v>644</v>
+      </c>
+      <c r="F42">
+        <v>470</v>
+      </c>
+      <c r="G42">
+        <v>7514</v>
+      </c>
+      <c r="H42">
+        <v>6</v>
+      </c>
+      <c r="I42">
+        <f>D42+E42+F42+G42</f>
+        <v>8635</v>
+      </c>
+      <c r="K42">
+        <v>784</v>
+      </c>
+      <c r="L42">
+        <v>37391</v>
+      </c>
+      <c r="M42">
+        <v>26266</v>
+      </c>
+      <c r="N42">
+        <f>K42+M42+L42*2</f>
+        <v>101832</v>
+      </c>
+      <c r="P42" s="3">
+        <v>6000</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>200</v>
+      </c>
+      <c r="R42" s="2">
+        <v>10</v>
+      </c>
+      <c r="S42" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="T42" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="U42" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>200</v>
+      </c>
+      <c r="C43">
+        <v>2016</v>
+      </c>
+      <c r="D43">
+        <v>864</v>
+      </c>
+      <c r="E43">
+        <v>50216</v>
+      </c>
+      <c r="F43">
+        <v>41352</v>
+      </c>
+      <c r="G43">
+        <v>27243</v>
+      </c>
+      <c r="H43">
+        <v>447</v>
+      </c>
+      <c r="I43">
+        <f>D43+E43+F43+G43</f>
+        <v>119675</v>
+      </c>
+      <c r="K43">
+        <v>4117</v>
+      </c>
+      <c r="L43">
+        <v>229057</v>
+      </c>
+      <c r="M43">
+        <v>210819</v>
+      </c>
+      <c r="N43">
+        <f>K43+M43+L43*2</f>
+        <v>673050</v>
+      </c>
+      <c r="P43" s="3">
+        <v>6000</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>200</v>
+      </c>
+      <c r="R43" s="2">
+        <v>200</v>
+      </c>
+      <c r="S43" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="T43" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="U43" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44">
+        <v>200</v>
+      </c>
+      <c r="C44">
+        <v>6283</v>
+      </c>
+      <c r="D44">
+        <v>19</v>
+      </c>
+      <c r="E44">
+        <v>3202</v>
+      </c>
+      <c r="F44">
+        <v>8800</v>
+      </c>
+      <c r="G44">
+        <v>51924</v>
+      </c>
+      <c r="H44">
+        <v>9</v>
+      </c>
+      <c r="I44">
+        <f>D44+E44+F44+G44</f>
+        <v>63945</v>
+      </c>
+      <c r="K44">
+        <v>978</v>
+      </c>
+      <c r="L44">
+        <v>185458</v>
+      </c>
+      <c r="M44">
+        <v>174352</v>
+      </c>
+      <c r="N44">
+        <f>K44+M44+L44*2</f>
+        <v>546246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
+      <c r="A45">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>117</v>
+      </c>
+      <c r="C45">
+        <v>6307</v>
+      </c>
+      <c r="D45">
+        <v>62</v>
+      </c>
+      <c r="E45">
+        <v>4638</v>
+      </c>
+      <c r="F45">
+        <v>4326</v>
+      </c>
+      <c r="G45">
+        <v>1274</v>
+      </c>
+      <c r="H45">
+        <v>49</v>
+      </c>
+      <c r="I45">
+        <f>D45+E45+F45+G45</f>
+        <v>10300</v>
+      </c>
+      <c r="K45">
+        <v>3415</v>
+      </c>
+      <c r="L45">
+        <v>31908</v>
+      </c>
+      <c r="M45">
+        <v>8189</v>
+      </c>
+      <c r="N45">
+        <f>K45+M45+L45*2</f>
+        <v>75420</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
+      <c r="A47" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47">
+        <f>200 * 15 + 8 * 70 + 10 * 5 + 150 + 50</f>
+        <v>3810</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14">
+      <c r="B49" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14">
+      <c r="B50" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14">
+      <c r="B51" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14">
+      <c r="B52" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14">
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>72</v>
+      </c>
+      <c r="G54" t="s">
+        <v>69</v>
+      </c>
+      <c r="H54" t="s">
+        <v>73</v>
+      </c>
+      <c r="I54" t="s">
+        <v>70</v>
+      </c>
+      <c r="K54" t="s">
+        <v>98</v>
+      </c>
+      <c r="L54" t="s">
+        <v>99</v>
+      </c>
+      <c r="M54" t="s">
+        <v>100</v>
+      </c>
+      <c r="N54" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14">
+      <c r="B55">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14">
+      <c r="B56">
+        <v>100</v>
+      </c>
+      <c r="D56" t="s">
+        <v>112</v>
+      </c>
+      <c r="I56" t="e">
+        <f>D56+E56+F56+G56</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N56">
+        <f>K56+M56+L56*2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14">
+      <c r="B58" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14">
+      <c r="B59" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14">
+      <c r="B60" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="61" spans="2:14">
+      <c r="B61" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14">
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>109</v>
+      </c>
+      <c r="D63" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
+        <v>72</v>
+      </c>
+      <c r="G63" t="s">
+        <v>69</v>
+      </c>
+      <c r="H63" t="s">
+        <v>73</v>
+      </c>
+      <c r="I63" t="s">
+        <v>70</v>
+      </c>
+      <c r="K63" t="s">
+        <v>98</v>
+      </c>
+      <c r="L63" t="s">
+        <v>99</v>
+      </c>
+      <c r="M63" t="s">
+        <v>100</v>
+      </c>
+      <c r="N63" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14">
+      <c r="B64">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="2:14">
+      <c r="B65">
+        <v>100</v>
+      </c>
+      <c r="D65" t="s">
+        <v>112</v>
+      </c>
+      <c r="I65" t="e">
+        <f>D65+E65+F65+G65</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N65">
+        <f>K65+M65+L65*2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:14">
+      <c r="B68" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="69" spans="2:14">
+      <c r="B69" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="70" spans="2:14">
+      <c r="B70" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14">
+      <c r="B71" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="73" spans="2:14">
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" t="s">
+        <v>109</v>
+      </c>
+      <c r="D73" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>1</v>
+      </c>
+      <c r="F73" t="s">
+        <v>72</v>
+      </c>
+      <c r="G73" t="s">
+        <v>69</v>
+      </c>
+      <c r="H73" t="s">
+        <v>73</v>
+      </c>
+      <c r="I73" t="s">
+        <v>70</v>
+      </c>
+      <c r="K73" t="s">
+        <v>98</v>
+      </c>
+      <c r="L73" t="s">
+        <v>99</v>
+      </c>
+      <c r="M73" t="s">
+        <v>100</v>
+      </c>
+      <c r="N73" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14">
+      <c r="B74">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="2:14">
+      <c r="B75">
+        <v>100</v>
+      </c>
+      <c r="N75">
+        <f>K75+M75+L75*2</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="3"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" t="s">
+        <v>99</v>
+      </c>
+      <c r="M4" t="s">
+        <v>100</v>
+      </c>
+      <c r="N4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="B6">
+        <v>200</v>
+      </c>
+      <c r="C6">
+        <v>200</v>
+      </c>
+      <c r="D6">
+        <v>4973</v>
+      </c>
+      <c r="E6">
+        <v>110126</v>
+      </c>
+      <c r="F6">
+        <v>150</v>
+      </c>
+      <c r="G6">
+        <v>116971</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <f>D6+E6+F6+G6</f>
+        <v>232220</v>
+      </c>
+      <c r="K6">
+        <v>5564</v>
+      </c>
+      <c r="L6">
+        <v>210642</v>
+      </c>
+      <c r="M6">
+        <v>195368</v>
+      </c>
+      <c r="N6">
+        <f>K6+M6+L6*2</f>
+        <v>622216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="D7">
+        <v>3544</v>
+      </c>
+      <c r="E7">
+        <v>106043</v>
+      </c>
+      <c r="F7">
+        <v>138</v>
+      </c>
+      <c r="G7">
+        <v>111612</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <f>D7+E7+F7+G7</f>
+        <v>221337</v>
+      </c>
+      <c r="K7">
+        <v>3946</v>
+      </c>
+      <c r="L7">
+        <v>198515</v>
+      </c>
+      <c r="M7">
+        <v>186537</v>
+      </c>
+      <c r="N7">
+        <f>K7+M7+L7*2</f>
+        <v>587513</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="D8">
+        <v>34</v>
+      </c>
+      <c r="E8">
+        <v>89109</v>
+      </c>
+      <c r="F8">
+        <v>139</v>
+      </c>
+      <c r="G8">
+        <v>109624</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <f>D8+E8+F8+G8</f>
+        <v>198906</v>
+      </c>
+      <c r="K8">
+        <v>272</v>
+      </c>
+      <c r="L8">
+        <v>180071</v>
+      </c>
+      <c r="M8">
+        <v>171842</v>
+      </c>
+      <c r="N8">
+        <f>K8+M8+L8*2</f>
+        <v>532256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="I10" s="2">
+        <f>(I6+I7+I8)/3</f>
+        <v>217487.66666666666</v>
+      </c>
+      <c r="N10" s="2">
+        <f>(N6+N7+N8)/3</f>
+        <v>580661.66666666663</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K14" t="s">
+        <v>98</v>
+      </c>
+      <c r="L14" t="s">
+        <v>99</v>
+      </c>
+      <c r="M14" t="s">
+        <v>100</v>
+      </c>
+      <c r="N14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16">
+        <v>200</v>
+      </c>
+      <c r="C16">
+        <v>200</v>
+      </c>
+      <c r="D16">
+        <v>32</v>
+      </c>
+      <c r="E16">
+        <v>2738</v>
+      </c>
+      <c r="F16">
+        <v>3170</v>
+      </c>
+      <c r="G16">
+        <v>9946</v>
+      </c>
+      <c r="H16">
+        <v>22</v>
+      </c>
+      <c r="I16">
+        <f>D16+E16+F16+G16</f>
+        <v>15886</v>
+      </c>
+      <c r="K16">
+        <v>1045</v>
+      </c>
+      <c r="L16">
+        <v>300509</v>
+      </c>
+      <c r="M16">
+        <v>155989</v>
+      </c>
+      <c r="N16">
+        <f>K16+M16+L16*2</f>
+        <v>758052</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>50</v>
+      </c>
+      <c r="D18">
+        <v>81</v>
+      </c>
+      <c r="E18">
+        <v>13953</v>
+      </c>
+      <c r="F18">
+        <v>118</v>
+      </c>
+      <c r="G18">
+        <v>3157</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <f>D18+E18+F18+G18</f>
+        <v>17309</v>
+      </c>
+      <c r="K18">
+        <v>142</v>
+      </c>
+      <c r="L18">
+        <v>24126</v>
+      </c>
+      <c r="M18">
+        <v>10099</v>
+      </c>
+      <c r="N18">
+        <f>K18+M18+L18*2</f>
+        <v>58493</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="D19">
+        <v>100</v>
+      </c>
+      <c r="E19">
+        <v>7091</v>
+      </c>
+      <c r="F19">
+        <v>194</v>
+      </c>
+      <c r="G19">
+        <v>3482</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <f>D19+E19+F19+G19</f>
+        <v>10867</v>
+      </c>
+      <c r="K19">
+        <v>195</v>
+      </c>
+      <c r="L19">
+        <v>10153</v>
+      </c>
+      <c r="M19">
+        <v>5071</v>
+      </c>
+      <c r="N19">
+        <f>K19+M19+L19*2</f>
+        <v>25572</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="D20">
+        <v>87</v>
+      </c>
+      <c r="E20">
+        <v>7285</v>
+      </c>
+      <c r="F20">
+        <v>159</v>
+      </c>
+      <c r="G20">
+        <v>3615</v>
+      </c>
+      <c r="H20">
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <f>D20+E20+F20+G20</f>
+        <v>11146</v>
+      </c>
+      <c r="K20">
+        <v>144</v>
+      </c>
+      <c r="L20">
+        <v>10756</v>
+      </c>
+      <c r="M20">
+        <v>5078</v>
+      </c>
+      <c r="N20">
+        <f>K20+M20+L20*2</f>
+        <v>26734</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="I21" s="2">
+        <f>(I20+I18+I19)/3</f>
+        <v>13107.333333333334</v>
+      </c>
+      <c r="N21" s="2">
+        <f>(N20+N18+N19)/3</f>
+        <v>36933</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23">
+        <v>200</v>
+      </c>
+      <c r="C23">
+        <v>200</v>
+      </c>
+      <c r="D23">
+        <v>41</v>
+      </c>
+      <c r="E23">
+        <v>50600</v>
+      </c>
+      <c r="F23">
+        <v>154</v>
+      </c>
+      <c r="G23">
+        <v>48455</v>
+      </c>
+      <c r="H23">
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <f>D23+E23+F23+G23</f>
+        <v>99250</v>
+      </c>
+      <c r="K23">
+        <v>202</v>
+      </c>
+      <c r="L23">
+        <v>110815</v>
+      </c>
+      <c r="M23">
+        <v>85874</v>
+      </c>
+      <c r="N23">
+        <f>K23+M23+L23*2</f>
+        <v>307706</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="D24">
+        <v>3744</v>
+      </c>
+      <c r="E24">
+        <v>48183</v>
+      </c>
+      <c r="F24">
+        <v>253</v>
+      </c>
+      <c r="G24">
+        <v>44776</v>
+      </c>
+      <c r="H24">
+        <v>8</v>
+      </c>
+      <c r="I24">
+        <f>D24+E24+F24+G24</f>
+        <v>96956</v>
+      </c>
+      <c r="K24">
+        <v>4002</v>
+      </c>
+      <c r="L24">
+        <v>98537</v>
+      </c>
+      <c r="M24">
+        <v>84740</v>
+      </c>
+      <c r="N24">
+        <f>K24+M24+L24*2</f>
+        <v>285816</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="D25">
+        <v>22</v>
+      </c>
+      <c r="E25">
+        <v>45817</v>
+      </c>
+      <c r="F25">
+        <v>217</v>
+      </c>
+      <c r="G25">
+        <v>44735</v>
+      </c>
+      <c r="H25">
+        <v>7</v>
+      </c>
+      <c r="I25">
+        <f>D25+E25+F25+G25</f>
+        <v>90791</v>
+      </c>
+      <c r="K25">
+        <v>156</v>
+      </c>
+      <c r="L25">
+        <v>95149</v>
+      </c>
+      <c r="M25">
+        <v>79952</v>
+      </c>
+      <c r="N25">
+        <f>K25+M25+L25*2</f>
+        <v>270406</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="I26" s="2">
+        <f>(I25+I23+I24)/3</f>
+        <v>95665.666666666672</v>
+      </c>
+      <c r="N26" s="2">
+        <f>(N25+N23+N24)/3</f>
+        <v>287976</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>